<commit_message>
Laboratorio 4 – Entrega final
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricau\Documents\Uniandes\EDA\LabSorts-S04-G07\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15b26424214f1033/Documents/4to semestre/Estructura de datos/Lab 4/LabSorts-S04-G07/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF92F0A7-35B5-405E-B007-FCA6AD7DA9DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="13_ncr:1_{FF92F0A7-35B5-405E-B007-FCA6AD7DA9DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{28BB8888-15AC-4C6C-A598-FC26095A20F5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <r>
       <t>T</t>
@@ -78,6 +78,9 @@
       </rPr>
       <t>amaño de la muestra (ARRAYLIST)</t>
     </r>
+  </si>
+  <si>
+    <t>17593.75</t>
   </si>
 </sst>
 </file>
@@ -130,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -142,6 +145,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,7 +468,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -526,7 +535,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +622,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -663,6 +672,21 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2969.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198375</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -721,8 +745,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -751,7 +774,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -801,6 +824,21 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>796.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3421.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14359.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>222703.12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -888,7 +926,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -938,6 +976,33 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>515.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1203.1199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2723.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7333.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17960.937000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38781.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -963,6 +1028,8 @@
         <c:axId val="696671312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1036,7 +1103,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1074,7 +1141,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1085,6 +1152,7 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1158,7 +1226,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1196,7 +1264,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1238,7 +1306,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1275,7 +1343,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1284,7 +1352,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1351,7 +1419,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1409,9 +1477,10 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
             <c:trendlineLbl>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
@@ -1438,7 +1507,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1488,6 +1557,12 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>56906.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>475468.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1546,8 +1621,128 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50218.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>419000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50218.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>419000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E4D7-4455-A92B-E398EC107F76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Datos Lab4'!$D$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell Sort [ms]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -1576,114 +1771,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E4D7-4455-A92B-E398EC107F76}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Datos Lab4'!$D$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Shell Sort [ms]</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1733,6 +1821,18 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2921.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12765.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58093.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306562</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1758,6 +1858,8 @@
         <c:axId val="696671312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1831,7 +1933,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1869,7 +1971,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -1880,6 +1982,7 @@
         <c:axId val="1833162896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1953,11 +2056,11 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1991,7 +2094,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -2033,7 +2136,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2070,7 +2173,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2079,7 +2182,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2146,7 +2249,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2207,7 +2310,7 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
             <c:trendlineLbl>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
@@ -2234,7 +2337,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2284,6 +2387,21 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2969.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51078</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>198375</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2345,7 +2463,7 @@
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
             <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
+            <c:dispEq val="0"/>
             <c:trendlineLbl>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
@@ -2372,7 +2490,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2422,6 +2540,12 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>56906.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>475468.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2447,6 +2571,8 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2520,7 +2646,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2558,7 +2684,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -2637,7 +2763,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2675,7 +2801,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -2717,7 +2843,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2754,7 +2880,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -2763,7 +2889,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2825,7 +2951,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2913,7 +3039,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2963,6 +3089,21 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>796.875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3421.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14359.37</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>222703.12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3051,7 +3192,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3101,6 +3242,12 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50218.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>419000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3126,6 +3273,7 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3199,7 +3347,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3237,7 +3385,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3316,7 +3464,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3354,7 +3502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -3396,7 +3544,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3433,7 +3581,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -3442,7 +3590,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3504,7 +3652,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3563,7 +3711,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="4"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3592,7 +3740,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3642,6 +3790,33 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>31.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>515.62</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1203.1199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2723.95</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7333.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17960.937000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38781.25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3701,7 +3876,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -3730,7 +3905,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3780,6 +3955,18 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2921.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12765.62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58093.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>306562</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3805,6 +3992,8 @@
         <c:axId val="1328118000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="512000"/>
+          <c:min val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3878,7 +4067,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3916,7 +4105,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328121328"/>
@@ -3927,6 +4116,7 @@
         <c:axId val="1328121328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3995,7 +4185,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4033,7 +4223,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1328118000"/>
@@ -4075,7 +4265,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4112,7 +4302,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -6896,7 +7086,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="79" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6907,7 +7097,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0D09CF8B-80E2-4734-A9D4-9F6060F1BA3D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6918,7 +7108,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{3D4D373F-B89D-476A-916E-D6B8B50B0AC1}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="69" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6929,7 +7119,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{662C0436-FCD4-45AD-AA7D-093158D92847}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6940,7 +7130,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="89" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6951,7 +7141,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="9298112" cy="6070315"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6984,7 +7174,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9298112" cy="6070315"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7017,7 +7207,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9298112" cy="6070315"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7050,7 +7240,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="9298112" cy="6070315"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7083,7 +7273,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8668712" cy="6292273"/>
+    <xdr:ext cx="9298112" cy="6070315"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7139,7 +7329,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7435,21 +7625,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7463,79 +7653,186 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="6">
+        <v>750</v>
+      </c>
+      <c r="C2" s="6">
+        <v>796.875</v>
+      </c>
+      <c r="D2" s="4">
+        <v>31.25</v>
+      </c>
+      <c r="N2">
+        <v>31.25</v>
+      </c>
+      <c r="O2">
+        <v>31.25</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="4">
+        <v>2969.75</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3421.875</v>
+      </c>
+      <c r="D3" s="4">
+        <v>98.96</v>
+      </c>
+      <c r="N3">
+        <v>78.125</v>
+      </c>
+      <c r="O3">
+        <v>93.75</v>
+      </c>
+      <c r="P3">
+        <v>125</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="4">
+        <v>12250</v>
+      </c>
+      <c r="C4" s="4">
+        <v>14359.37</v>
+      </c>
+      <c r="D4" s="4">
+        <v>192.7</v>
+      </c>
+      <c r="N4">
+        <v>187.5</v>
+      </c>
+      <c r="O4">
+        <v>187.5</v>
+      </c>
+      <c r="P4">
+        <v>203.125</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="4">
+        <v>51078</v>
+      </c>
+      <c r="C5" s="4">
+        <v>58250</v>
+      </c>
+      <c r="D5" s="4">
+        <v>515.62</v>
+      </c>
+      <c r="N5">
+        <v>500</v>
+      </c>
+      <c r="O5">
+        <v>484.375</v>
+      </c>
+      <c r="P5">
+        <v>562.5</v>
+      </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:16">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4">
+        <v>198375</v>
+      </c>
+      <c r="C6" s="4">
+        <v>222703.12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1203.1199999999999</v>
+      </c>
+      <c r="N6">
+        <v>1171.8699999999999</v>
+      </c>
+      <c r="O6">
+        <v>1203.1199999999999</v>
+      </c>
+      <c r="P6">
+        <v>1234.3699999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:16">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>2723.95</v>
+      </c>
+      <c r="N7">
+        <v>2562.5</v>
+      </c>
+      <c r="O7">
+        <v>2796.87</v>
+      </c>
+      <c r="P7">
+        <v>2812.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:16">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>7333.33</v>
+      </c>
+      <c r="N8">
+        <v>7296.87</v>
+      </c>
+      <c r="O8">
+        <v>7343.75</v>
+      </c>
+      <c r="P8">
+        <v>7359.375</v>
+      </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:16">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>17960.937000000002</v>
+      </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:16">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>38781.25</v>
+      </c>
+      <c r="N10">
+        <v>17828.125</v>
+      </c>
+      <c r="O10">
+        <v>18093.75</v>
+      </c>
+      <c r="P10" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:16">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
@@ -7543,7 +7840,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -7557,21 +7854,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:16">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="5">
+        <v>56906.25</v>
+      </c>
+      <c r="C15" s="4">
+        <v>50218.75</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2921.87</v>
+      </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:16">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="4">
+        <v>475468.75</v>
+      </c>
+      <c r="C16" s="4">
+        <v>419000</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12765.62</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
@@ -7579,7 +7888,9 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4">
+        <v>58093.75</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
@@ -7587,7 +7898,9 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4">
+        <v>306562</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">

</xml_diff>